<commit_message>
Commit 11: ajuste da margem nas telas, após teste com turmas grandes, correção do calculo de presença
</commit_message>
<xml_diff>
--- a/Teste/teste_alunos.xlsx
+++ b/Teste/teste_alunos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2947685926b3e492/Documentos/GitHub/UNIVESP-PI-Sistema_Gerenciador_de_Atrasos/Teste/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{9E1B8C18-654C-4898-98C4-BD658677F0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6607E2B8-0065-4196-AEE9-5F79272D1284}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{9E1B8C18-654C-4898-98C4-BD658677F0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4646614-DDAB-47A4-88D2-A319D0386D11}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{077E4775-C7D5-400F-B51C-35EADCF32792}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="329">
   <si>
     <t>R.A.</t>
   </si>
@@ -167,13 +167,853 @@
   </si>
   <si>
     <t>Responsável 2</t>
+  </si>
+  <si>
+    <t>Aluno 11</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 11</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 11</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 11</t>
+  </si>
+  <si>
+    <t>Aluno 12</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 12</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 12</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 12</t>
+  </si>
+  <si>
+    <t>Aluno 13</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 13</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 13</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 13</t>
+  </si>
+  <si>
+    <t>Aluno 14</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 14</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 14</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 14</t>
+  </si>
+  <si>
+    <t>Aluno 15</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 15</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 15</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 15</t>
+  </si>
+  <si>
+    <t>Aluno 16</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 16</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 16</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 16</t>
+  </si>
+  <si>
+    <t>Aluno 17</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 17</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 17</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 17</t>
+  </si>
+  <si>
+    <t>Aluno 18</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 18</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 18</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 18</t>
+  </si>
+  <si>
+    <t>Aluno 19</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 19</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 19</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 19</t>
+  </si>
+  <si>
+    <t>Aluno 20</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 20</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 20</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 20</t>
+  </si>
+  <si>
+    <t>Aluno 21</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 21</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 21</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 21</t>
+  </si>
+  <si>
+    <t>Aluno 22</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 22</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 22</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 22</t>
+  </si>
+  <si>
+    <t>Aluno 23</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 23</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 23</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 23</t>
+  </si>
+  <si>
+    <t>Aluno 24</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 24</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 24</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 24</t>
+  </si>
+  <si>
+    <t>Aluno 25</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 25</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 25</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 25</t>
+  </si>
+  <si>
+    <t>Aluno 26</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 26</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 26</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 26</t>
+  </si>
+  <si>
+    <t>Aluno 27</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 27</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 27</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 27</t>
+  </si>
+  <si>
+    <t>Aluno 28</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 28</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 28</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 28</t>
+  </si>
+  <si>
+    <t>Aluno 29</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 29</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 29</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 29</t>
+  </si>
+  <si>
+    <t>Aluno 30</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 30</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 30</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 30</t>
+  </si>
+  <si>
+    <t>Aluno 31</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 31</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 31</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 31</t>
+  </si>
+  <si>
+    <t>Aluno 32</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 32</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 32</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 32</t>
+  </si>
+  <si>
+    <t>Aluno 33</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 33</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 33</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 33</t>
+  </si>
+  <si>
+    <t>Aluno 34</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 34</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 34</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 34</t>
+  </si>
+  <si>
+    <t>Aluno 35</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 35</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 35</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 35</t>
+  </si>
+  <si>
+    <t>Aluno 36</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 36</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 36</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 36</t>
+  </si>
+  <si>
+    <t>Aluno 37</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 37</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 37</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 37</t>
+  </si>
+  <si>
+    <t>Aluno 38</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 38</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 38</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 38</t>
+  </si>
+  <si>
+    <t>Aluno 39</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 39</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 39</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 39</t>
+  </si>
+  <si>
+    <t>Aluno 40</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 40</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 40</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 40</t>
+  </si>
+  <si>
+    <t>Aluno 41</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 41</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 41</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 41</t>
+  </si>
+  <si>
+    <t>Aluno 42</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 42</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 42</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 42</t>
+  </si>
+  <si>
+    <t>Aluno 43</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 43</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 43</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 43</t>
+  </si>
+  <si>
+    <t>Aluno 44</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 44</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 44</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 44</t>
+  </si>
+  <si>
+    <t>Aluno 45</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 45</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 45</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 45</t>
+  </si>
+  <si>
+    <t>Aluno 46</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 46</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 46</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 46</t>
+  </si>
+  <si>
+    <t>Aluno 47</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 47</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 47</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 47</t>
+  </si>
+  <si>
+    <t>Aluno 48</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 48</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 48</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 48</t>
+  </si>
+  <si>
+    <t>Aluno 49</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 49</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 49</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 49</t>
+  </si>
+  <si>
+    <t>Aluno 50</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 50</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 50</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 50</t>
+  </si>
+  <si>
+    <t>Aluno 51</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 51</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 51</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 51</t>
+  </si>
+  <si>
+    <t>Aluno 52</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 52</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 52</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 52</t>
+  </si>
+  <si>
+    <t>Aluno 53</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 53</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 53</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 53</t>
+  </si>
+  <si>
+    <t>Aluno 54</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 54</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 54</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 54</t>
+  </si>
+  <si>
+    <t>Aluno 55</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 55</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 55</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 55</t>
+  </si>
+  <si>
+    <t>Aluno 56</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 56</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 56</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 56</t>
+  </si>
+  <si>
+    <t>Aluno 57</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 57</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 57</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 57</t>
+  </si>
+  <si>
+    <t>Aluno 58</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 58</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 58</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 58</t>
+  </si>
+  <si>
+    <t>Aluno 59</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 59</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 59</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 59</t>
+  </si>
+  <si>
+    <t>Aluno 60</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 60</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 60</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 60</t>
+  </si>
+  <si>
+    <t>Aluno 61</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 61</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 61</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 61</t>
+  </si>
+  <si>
+    <t>Aluno 62</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 62</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 62</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 62</t>
+  </si>
+  <si>
+    <t>Aluno 63</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 63</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 63</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 63</t>
+  </si>
+  <si>
+    <t>Aluno 64</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 64</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 64</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 64</t>
+  </si>
+  <si>
+    <t>Aluno 65</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 65</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 65</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 65</t>
+  </si>
+  <si>
+    <t>Aluno 66</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 66</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 66</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 66</t>
+  </si>
+  <si>
+    <t>Aluno 67</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 67</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 67</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 67</t>
+  </si>
+  <si>
+    <t>Aluno 68</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 68</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 68</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 68</t>
+  </si>
+  <si>
+    <t>Aluno 69</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 69</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 69</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 69</t>
+  </si>
+  <si>
+    <t>Aluno 70</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 70</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 70</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 70</t>
+  </si>
+  <si>
+    <t>Aluno 71</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 71</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 71</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 71</t>
+  </si>
+  <si>
+    <t>Aluno 72</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 72</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 72</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 72</t>
+  </si>
+  <si>
+    <t>Aluno 73</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 73</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 73</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 73</t>
+  </si>
+  <si>
+    <t>Aluno 74</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 74</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 74</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 74</t>
+  </si>
+  <si>
+    <t>Aluno 75</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 75</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 75</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 75</t>
+  </si>
+  <si>
+    <t>Aluno 76</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 76</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 76</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 76</t>
+  </si>
+  <si>
+    <t>Aluno 77</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 77</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 77</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 77</t>
+  </si>
+  <si>
+    <t>Aluno 78</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 78</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 78</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 78</t>
+  </si>
+  <si>
+    <t>Aluno 79</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 79</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 79</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 79</t>
+  </si>
+  <si>
+    <t>Aluno 80</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 80</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 80</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 80</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +1144,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1031,10 +1877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8E3125-0512-415E-8725-BC38948E20FC}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42:C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1194,7 +2040,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>
@@ -1217,7 +2063,7 @@
         <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
         <v>32</v>
@@ -1240,7 +2086,7 @@
         <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
         <v>36</v>
@@ -1263,7 +2109,7 @@
         <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
         <v>40</v>
@@ -1286,7 +2132,7 @@
         <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
         <v>44</v>
@@ -1301,7 +2147,1618 @@
         <v>11987654330</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>202511</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12">
+        <v>11987654331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>202512</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13">
+        <v>11987654332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>202513</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14">
+        <v>11987654333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>202514</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15">
+        <v>11987654334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>202515</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16">
+        <v>11987654335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>202516</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17">
+        <v>11987654336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>202517</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18">
+        <v>11987654337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>202518</v>
+      </c>
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19">
+        <v>11987654338</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>202519</v>
+      </c>
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20">
+        <v>11987654339</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>202520</v>
+      </c>
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21">
+        <v>11987654340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>202521</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22">
+        <v>11987654341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>202522</v>
+      </c>
+      <c r="B23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23">
+        <v>11987654342</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>202523</v>
+      </c>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" t="s">
+        <v>100</v>
+      </c>
+      <c r="G24">
+        <v>11987654343</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>202524</v>
+      </c>
+      <c r="B25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25">
+        <v>11987654344</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>202525</v>
+      </c>
+      <c r="B26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26">
+        <v>11987654345</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>202526</v>
+      </c>
+      <c r="B27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27">
+        <v>11987654346</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>202527</v>
+      </c>
+      <c r="B28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28">
+        <v>11987654347</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>202528</v>
+      </c>
+      <c r="B29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" t="s">
+        <v>119</v>
+      </c>
+      <c r="F29" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29">
+        <v>11987654348</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>202529</v>
+      </c>
+      <c r="B30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" t="s">
+        <v>123</v>
+      </c>
+      <c r="F30" t="s">
+        <v>124</v>
+      </c>
+      <c r="G30">
+        <v>11987654349</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>202530</v>
+      </c>
+      <c r="B31" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>126</v>
+      </c>
+      <c r="E31" t="s">
+        <v>127</v>
+      </c>
+      <c r="F31" t="s">
+        <v>128</v>
+      </c>
+      <c r="G31">
+        <v>11987654350</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>202531</v>
+      </c>
+      <c r="B32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" t="s">
+        <v>131</v>
+      </c>
+      <c r="F32" t="s">
+        <v>132</v>
+      </c>
+      <c r="G32">
+        <v>11987654351</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>202532</v>
+      </c>
+      <c r="B33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>134</v>
+      </c>
+      <c r="E33" t="s">
+        <v>135</v>
+      </c>
+      <c r="F33" t="s">
+        <v>136</v>
+      </c>
+      <c r="G33">
+        <v>11987654352</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>202533</v>
+      </c>
+      <c r="B34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>138</v>
+      </c>
+      <c r="E34" t="s">
+        <v>139</v>
+      </c>
+      <c r="F34" t="s">
+        <v>140</v>
+      </c>
+      <c r="G34">
+        <v>11987654353</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>202534</v>
+      </c>
+      <c r="B35" t="s">
+        <v>141</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>142</v>
+      </c>
+      <c r="E35" t="s">
+        <v>143</v>
+      </c>
+      <c r="F35" t="s">
+        <v>144</v>
+      </c>
+      <c r="G35">
+        <v>11987654354</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>202535</v>
+      </c>
+      <c r="B36" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>146</v>
+      </c>
+      <c r="E36" t="s">
+        <v>147</v>
+      </c>
+      <c r="F36" t="s">
+        <v>148</v>
+      </c>
+      <c r="G36">
+        <v>11987654355</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>202536</v>
+      </c>
+      <c r="B37" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>150</v>
+      </c>
+      <c r="E37" t="s">
+        <v>151</v>
+      </c>
+      <c r="F37" t="s">
+        <v>152</v>
+      </c>
+      <c r="G37">
+        <v>11987654356</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>202537</v>
+      </c>
+      <c r="B38" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>154</v>
+      </c>
+      <c r="E38" t="s">
+        <v>155</v>
+      </c>
+      <c r="F38" t="s">
+        <v>156</v>
+      </c>
+      <c r="G38">
+        <v>11987654357</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>202538</v>
+      </c>
+      <c r="B39" t="s">
+        <v>157</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>158</v>
+      </c>
+      <c r="E39" t="s">
+        <v>159</v>
+      </c>
+      <c r="F39" t="s">
+        <v>160</v>
+      </c>
+      <c r="G39">
+        <v>11987654358</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>202539</v>
+      </c>
+      <c r="B40" t="s">
+        <v>161</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>162</v>
+      </c>
+      <c r="E40" t="s">
+        <v>163</v>
+      </c>
+      <c r="F40" t="s">
+        <v>164</v>
+      </c>
+      <c r="G40">
+        <v>11987654359</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>202540</v>
+      </c>
+      <c r="B41" t="s">
+        <v>165</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>166</v>
+      </c>
+      <c r="E41" t="s">
+        <v>167</v>
+      </c>
+      <c r="F41" t="s">
+        <v>168</v>
+      </c>
+      <c r="G41">
+        <v>11987654360</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>202541</v>
+      </c>
+      <c r="B42" t="s">
+        <v>169</v>
+      </c>
+      <c r="C42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E42" t="s">
+        <v>171</v>
+      </c>
+      <c r="F42" t="s">
+        <v>172</v>
+      </c>
+      <c r="G42">
+        <v>11987654361</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>202542</v>
+      </c>
+      <c r="B43" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" t="s">
+        <v>174</v>
+      </c>
+      <c r="E43" t="s">
+        <v>175</v>
+      </c>
+      <c r="F43" t="s">
+        <v>176</v>
+      </c>
+      <c r="G43">
+        <v>11987654362</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>202543</v>
+      </c>
+      <c r="B44" t="s">
+        <v>177</v>
+      </c>
+      <c r="C44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" t="s">
+        <v>178</v>
+      </c>
+      <c r="E44" t="s">
+        <v>179</v>
+      </c>
+      <c r="F44" t="s">
+        <v>180</v>
+      </c>
+      <c r="G44">
+        <v>11987654363</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>202544</v>
+      </c>
+      <c r="B45" t="s">
+        <v>181</v>
+      </c>
+      <c r="C45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" t="s">
+        <v>182</v>
+      </c>
+      <c r="E45" t="s">
+        <v>183</v>
+      </c>
+      <c r="F45" t="s">
+        <v>184</v>
+      </c>
+      <c r="G45">
+        <v>11987654364</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>202545</v>
+      </c>
+      <c r="B46" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" t="s">
+        <v>186</v>
+      </c>
+      <c r="E46" t="s">
+        <v>187</v>
+      </c>
+      <c r="F46" t="s">
+        <v>188</v>
+      </c>
+      <c r="G46">
+        <v>11987654365</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>202546</v>
+      </c>
+      <c r="B47" t="s">
+        <v>189</v>
+      </c>
+      <c r="C47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" t="s">
+        <v>190</v>
+      </c>
+      <c r="E47" t="s">
+        <v>191</v>
+      </c>
+      <c r="F47" t="s">
+        <v>192</v>
+      </c>
+      <c r="G47">
+        <v>11987654366</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>202547</v>
+      </c>
+      <c r="B48" t="s">
+        <v>193</v>
+      </c>
+      <c r="C48" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48" t="s">
+        <v>194</v>
+      </c>
+      <c r="E48" t="s">
+        <v>195</v>
+      </c>
+      <c r="F48" t="s">
+        <v>196</v>
+      </c>
+      <c r="G48">
+        <v>11987654367</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>202548</v>
+      </c>
+      <c r="B49" t="s">
+        <v>197</v>
+      </c>
+      <c r="C49" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" t="s">
+        <v>198</v>
+      </c>
+      <c r="E49" t="s">
+        <v>199</v>
+      </c>
+      <c r="F49" t="s">
+        <v>200</v>
+      </c>
+      <c r="G49">
+        <v>11987654368</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>202549</v>
+      </c>
+      <c r="B50" t="s">
+        <v>201</v>
+      </c>
+      <c r="C50" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" t="s">
+        <v>202</v>
+      </c>
+      <c r="E50" t="s">
+        <v>203</v>
+      </c>
+      <c r="F50" t="s">
+        <v>204</v>
+      </c>
+      <c r="G50">
+        <v>11987654369</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>202550</v>
+      </c>
+      <c r="B51" t="s">
+        <v>205</v>
+      </c>
+      <c r="C51" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" t="s">
+        <v>206</v>
+      </c>
+      <c r="E51" t="s">
+        <v>207</v>
+      </c>
+      <c r="F51" t="s">
+        <v>208</v>
+      </c>
+      <c r="G51">
+        <v>11987654370</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>202551</v>
+      </c>
+      <c r="B52" t="s">
+        <v>209</v>
+      </c>
+      <c r="C52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" t="s">
+        <v>210</v>
+      </c>
+      <c r="E52" t="s">
+        <v>211</v>
+      </c>
+      <c r="F52" t="s">
+        <v>212</v>
+      </c>
+      <c r="G52">
+        <v>11987654371</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>202552</v>
+      </c>
+      <c r="B53" t="s">
+        <v>213</v>
+      </c>
+      <c r="C53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53" t="s">
+        <v>214</v>
+      </c>
+      <c r="E53" t="s">
+        <v>215</v>
+      </c>
+      <c r="F53" t="s">
+        <v>216</v>
+      </c>
+      <c r="G53">
+        <v>11987654372</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>202553</v>
+      </c>
+      <c r="B54" t="s">
+        <v>217</v>
+      </c>
+      <c r="C54" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" t="s">
+        <v>218</v>
+      </c>
+      <c r="E54" t="s">
+        <v>219</v>
+      </c>
+      <c r="F54" t="s">
+        <v>220</v>
+      </c>
+      <c r="G54">
+        <v>11987654373</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>202554</v>
+      </c>
+      <c r="B55" t="s">
+        <v>221</v>
+      </c>
+      <c r="C55" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" t="s">
+        <v>222</v>
+      </c>
+      <c r="E55" t="s">
+        <v>223</v>
+      </c>
+      <c r="F55" t="s">
+        <v>224</v>
+      </c>
+      <c r="G55">
+        <v>11987654374</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>202555</v>
+      </c>
+      <c r="B56" t="s">
+        <v>225</v>
+      </c>
+      <c r="C56" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" t="s">
+        <v>226</v>
+      </c>
+      <c r="E56" t="s">
+        <v>227</v>
+      </c>
+      <c r="F56" t="s">
+        <v>228</v>
+      </c>
+      <c r="G56">
+        <v>11987654375</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>202556</v>
+      </c>
+      <c r="B57" t="s">
+        <v>229</v>
+      </c>
+      <c r="C57" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" t="s">
+        <v>230</v>
+      </c>
+      <c r="E57" t="s">
+        <v>231</v>
+      </c>
+      <c r="F57" t="s">
+        <v>232</v>
+      </c>
+      <c r="G57">
+        <v>11987654376</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>202557</v>
+      </c>
+      <c r="B58" t="s">
+        <v>233</v>
+      </c>
+      <c r="C58" t="s">
+        <v>27</v>
+      </c>
+      <c r="D58" t="s">
+        <v>234</v>
+      </c>
+      <c r="E58" t="s">
+        <v>235</v>
+      </c>
+      <c r="F58" t="s">
+        <v>236</v>
+      </c>
+      <c r="G58">
+        <v>11987654377</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>202558</v>
+      </c>
+      <c r="B59" t="s">
+        <v>237</v>
+      </c>
+      <c r="C59" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" t="s">
+        <v>238</v>
+      </c>
+      <c r="E59" t="s">
+        <v>239</v>
+      </c>
+      <c r="F59" t="s">
+        <v>240</v>
+      </c>
+      <c r="G59">
+        <v>11987654378</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>202559</v>
+      </c>
+      <c r="B60" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60" t="s">
+        <v>27</v>
+      </c>
+      <c r="D60" t="s">
+        <v>242</v>
+      </c>
+      <c r="E60" t="s">
+        <v>243</v>
+      </c>
+      <c r="F60" t="s">
+        <v>244</v>
+      </c>
+      <c r="G60">
+        <v>11987654379</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>202560</v>
+      </c>
+      <c r="B61" t="s">
+        <v>245</v>
+      </c>
+      <c r="C61" t="s">
+        <v>27</v>
+      </c>
+      <c r="D61" t="s">
+        <v>246</v>
+      </c>
+      <c r="E61" t="s">
+        <v>247</v>
+      </c>
+      <c r="F61" t="s">
+        <v>248</v>
+      </c>
+      <c r="G61">
+        <v>11987654380</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>202561</v>
+      </c>
+      <c r="B62" t="s">
+        <v>249</v>
+      </c>
+      <c r="C62" t="s">
+        <v>27</v>
+      </c>
+      <c r="D62" t="s">
+        <v>250</v>
+      </c>
+      <c r="E62" t="s">
+        <v>251</v>
+      </c>
+      <c r="F62" t="s">
+        <v>252</v>
+      </c>
+      <c r="G62">
+        <v>11987654381</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>202562</v>
+      </c>
+      <c r="B63" t="s">
+        <v>253</v>
+      </c>
+      <c r="C63" t="s">
+        <v>27</v>
+      </c>
+      <c r="D63" t="s">
+        <v>254</v>
+      </c>
+      <c r="E63" t="s">
+        <v>255</v>
+      </c>
+      <c r="F63" t="s">
+        <v>256</v>
+      </c>
+      <c r="G63">
+        <v>11987654382</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>202563</v>
+      </c>
+      <c r="B64" t="s">
+        <v>257</v>
+      </c>
+      <c r="C64" t="s">
+        <v>27</v>
+      </c>
+      <c r="D64" t="s">
+        <v>258</v>
+      </c>
+      <c r="E64" t="s">
+        <v>259</v>
+      </c>
+      <c r="F64" t="s">
+        <v>260</v>
+      </c>
+      <c r="G64">
+        <v>11987654383</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>202564</v>
+      </c>
+      <c r="B65" t="s">
+        <v>261</v>
+      </c>
+      <c r="C65" t="s">
+        <v>27</v>
+      </c>
+      <c r="D65" t="s">
+        <v>262</v>
+      </c>
+      <c r="E65" t="s">
+        <v>263</v>
+      </c>
+      <c r="F65" t="s">
+        <v>264</v>
+      </c>
+      <c r="G65">
+        <v>11987654384</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>202565</v>
+      </c>
+      <c r="B66" t="s">
+        <v>265</v>
+      </c>
+      <c r="C66" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" t="s">
+        <v>266</v>
+      </c>
+      <c r="E66" t="s">
+        <v>267</v>
+      </c>
+      <c r="F66" t="s">
+        <v>268</v>
+      </c>
+      <c r="G66">
+        <v>11987654385</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>202566</v>
+      </c>
+      <c r="B67" t="s">
+        <v>269</v>
+      </c>
+      <c r="C67" t="s">
+        <v>27</v>
+      </c>
+      <c r="D67" t="s">
+        <v>270</v>
+      </c>
+      <c r="E67" t="s">
+        <v>271</v>
+      </c>
+      <c r="F67" t="s">
+        <v>272</v>
+      </c>
+      <c r="G67">
+        <v>11987654386</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>202567</v>
+      </c>
+      <c r="B68" t="s">
+        <v>273</v>
+      </c>
+      <c r="C68" t="s">
+        <v>27</v>
+      </c>
+      <c r="D68" t="s">
+        <v>274</v>
+      </c>
+      <c r="E68" t="s">
+        <v>275</v>
+      </c>
+      <c r="F68" t="s">
+        <v>276</v>
+      </c>
+      <c r="G68">
+        <v>11987654387</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>202568</v>
+      </c>
+      <c r="B69" t="s">
+        <v>277</v>
+      </c>
+      <c r="C69" t="s">
+        <v>27</v>
+      </c>
+      <c r="D69" t="s">
+        <v>278</v>
+      </c>
+      <c r="E69" t="s">
+        <v>279</v>
+      </c>
+      <c r="F69" t="s">
+        <v>280</v>
+      </c>
+      <c r="G69">
+        <v>11987654388</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>202569</v>
+      </c>
+      <c r="B70" t="s">
+        <v>281</v>
+      </c>
+      <c r="C70" t="s">
+        <v>27</v>
+      </c>
+      <c r="D70" t="s">
+        <v>282</v>
+      </c>
+      <c r="E70" t="s">
+        <v>283</v>
+      </c>
+      <c r="F70" t="s">
+        <v>284</v>
+      </c>
+      <c r="G70">
+        <v>11987654389</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>202570</v>
+      </c>
+      <c r="B71" t="s">
+        <v>285</v>
+      </c>
+      <c r="C71" t="s">
+        <v>27</v>
+      </c>
+      <c r="D71" t="s">
+        <v>286</v>
+      </c>
+      <c r="E71" t="s">
+        <v>287</v>
+      </c>
+      <c r="F71" t="s">
+        <v>288</v>
+      </c>
+      <c r="G71">
+        <v>11987654390</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>202571</v>
+      </c>
+      <c r="B72" t="s">
+        <v>289</v>
+      </c>
+      <c r="C72" t="s">
+        <v>27</v>
+      </c>
+      <c r="D72" t="s">
+        <v>290</v>
+      </c>
+      <c r="E72" t="s">
+        <v>291</v>
+      </c>
+      <c r="F72" t="s">
+        <v>292</v>
+      </c>
+      <c r="G72">
+        <v>11987654391</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>202572</v>
+      </c>
+      <c r="B73" t="s">
+        <v>293</v>
+      </c>
+      <c r="C73" t="s">
+        <v>27</v>
+      </c>
+      <c r="D73" t="s">
+        <v>294</v>
+      </c>
+      <c r="E73" t="s">
+        <v>295</v>
+      </c>
+      <c r="F73" t="s">
+        <v>296</v>
+      </c>
+      <c r="G73">
+        <v>11987654392</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>202573</v>
+      </c>
+      <c r="B74" t="s">
+        <v>297</v>
+      </c>
+      <c r="C74" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" t="s">
+        <v>298</v>
+      </c>
+      <c r="E74" t="s">
+        <v>299</v>
+      </c>
+      <c r="F74" t="s">
+        <v>300</v>
+      </c>
+      <c r="G74">
+        <v>11987654393</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>202574</v>
+      </c>
+      <c r="B75" t="s">
+        <v>301</v>
+      </c>
+      <c r="C75" t="s">
+        <v>27</v>
+      </c>
+      <c r="D75" t="s">
+        <v>302</v>
+      </c>
+      <c r="E75" t="s">
+        <v>303</v>
+      </c>
+      <c r="F75" t="s">
+        <v>304</v>
+      </c>
+      <c r="G75">
+        <v>11987654394</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>202575</v>
+      </c>
+      <c r="B76" t="s">
+        <v>305</v>
+      </c>
+      <c r="C76" t="s">
+        <v>27</v>
+      </c>
+      <c r="D76" t="s">
+        <v>306</v>
+      </c>
+      <c r="E76" t="s">
+        <v>307</v>
+      </c>
+      <c r="F76" t="s">
+        <v>308</v>
+      </c>
+      <c r="G76">
+        <v>11987654395</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>202576</v>
+      </c>
+      <c r="B77" t="s">
+        <v>309</v>
+      </c>
+      <c r="C77" t="s">
+        <v>27</v>
+      </c>
+      <c r="D77" t="s">
+        <v>310</v>
+      </c>
+      <c r="E77" t="s">
+        <v>311</v>
+      </c>
+      <c r="F77" t="s">
+        <v>312</v>
+      </c>
+      <c r="G77">
+        <v>11987654396</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>202577</v>
+      </c>
+      <c r="B78" t="s">
+        <v>313</v>
+      </c>
+      <c r="C78" t="s">
+        <v>27</v>
+      </c>
+      <c r="D78" t="s">
+        <v>314</v>
+      </c>
+      <c r="E78" t="s">
+        <v>315</v>
+      </c>
+      <c r="F78" t="s">
+        <v>316</v>
+      </c>
+      <c r="G78">
+        <v>11987654397</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>202578</v>
+      </c>
+      <c r="B79" t="s">
+        <v>317</v>
+      </c>
+      <c r="C79" t="s">
+        <v>27</v>
+      </c>
+      <c r="D79" t="s">
+        <v>318</v>
+      </c>
+      <c r="E79" t="s">
+        <v>319</v>
+      </c>
+      <c r="F79" t="s">
+        <v>320</v>
+      </c>
+      <c r="G79">
+        <v>11987654398</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>202579</v>
+      </c>
+      <c r="B80" t="s">
+        <v>321</v>
+      </c>
+      <c r="C80" t="s">
+        <v>27</v>
+      </c>
+      <c r="D80" t="s">
+        <v>322</v>
+      </c>
+      <c r="E80" t="s">
+        <v>323</v>
+      </c>
+      <c r="F80" t="s">
+        <v>324</v>
+      </c>
+      <c r="G80">
+        <v>11987654399</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>202580</v>
+      </c>
+      <c r="B81" t="s">
+        <v>325</v>
+      </c>
+      <c r="C81" t="s">
+        <v>27</v>
+      </c>
+      <c r="D81" t="s">
+        <v>326</v>
+      </c>
+      <c r="E81" t="s">
+        <v>327</v>
+      </c>
+      <c r="F81" t="s">
+        <v>328</v>
+      </c>
+      <c r="G81">
+        <v>11987654400</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit 12: limitado o botão de limpar banco de dados aos usuarios administradores
</commit_message>
<xml_diff>
--- a/Teste/teste_alunos.xlsx
+++ b/Teste/teste_alunos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2947685926b3e492/Documentos/GitHub/UNIVESP-PI-Sistema_Gerenciador_de_Atrasos/Teste/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{9E1B8C18-654C-4898-98C4-BD658677F0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4646614-DDAB-47A4-88D2-A319D0386D11}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{9E1B8C18-654C-4898-98C4-BD658677F0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{677C196D-4834-4EC2-BF23-C97B69B62079}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{077E4775-C7D5-400F-B51C-35EADCF32792}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="333">
   <si>
     <t>R.A.</t>
   </si>
@@ -1007,6 +1007,18 @@
   </si>
   <si>
     <t>Mãe do Aluno 80</t>
+  </si>
+  <si>
+    <t>Aluno 161</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 161</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 161</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 161</t>
   </si>
 </sst>
 </file>
@@ -1877,10 +1889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8E3125-0512-415E-8725-BC38948E20FC}">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42:C81"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3757,6 +3769,29 @@
         <v>11987654400</v>
       </c>
     </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>202650</v>
+      </c>
+      <c r="B82" t="s">
+        <v>329</v>
+      </c>
+      <c r="C82" t="s">
+        <v>27</v>
+      </c>
+      <c r="D82" t="s">
+        <v>330</v>
+      </c>
+      <c r="E82" t="s">
+        <v>331</v>
+      </c>
+      <c r="F82" t="s">
+        <v>332</v>
+      </c>
+      <c r="G82">
+        <v>11987654499</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>